<commit_message>
mega form/alola form name data added
</commit_message>
<xml_diff>
--- a/alola_form.xlsx
+++ b/alola_form.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25516"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14720" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14740" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="工作表1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="80">
   <si>
     <t>HP</t>
   </si>
@@ -159,6 +159,122 @@
   <si>
     <t>type</t>
     <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>chName</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Name</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Alola Rattata</t>
+  </si>
+  <si>
+    <t>Alola Raticate</t>
+  </si>
+  <si>
+    <t>Alola Raichu</t>
+  </si>
+  <si>
+    <t>Alola Sandshrew</t>
+  </si>
+  <si>
+    <t>Alola Sandslash</t>
+  </si>
+  <si>
+    <t>Alola Vulpix</t>
+  </si>
+  <si>
+    <t>Alola Ninetales</t>
+  </si>
+  <si>
+    <t>Alola Diglett</t>
+  </si>
+  <si>
+    <t>Alola Dugtrio</t>
+  </si>
+  <si>
+    <t>Alola Meowth</t>
+  </si>
+  <si>
+    <t>Alola Persian</t>
+  </si>
+  <si>
+    <t>Alola Geodude</t>
+  </si>
+  <si>
+    <t>Alola Graveler</t>
+  </si>
+  <si>
+    <t>Alola Golem</t>
+  </si>
+  <si>
+    <t>Alola Grimer</t>
+  </si>
+  <si>
+    <t>Alola Muk</t>
+  </si>
+  <si>
+    <t>Alola Exeggutor</t>
+  </si>
+  <si>
+    <t>Alola Marowak</t>
+  </si>
+  <si>
+    <t>阿罗拉小拉达</t>
+  </si>
+  <si>
+    <t>阿罗拉拉达</t>
+  </si>
+  <si>
+    <t>阿罗拉雷丘</t>
+  </si>
+  <si>
+    <t>阿罗拉穿山鼠</t>
+  </si>
+  <si>
+    <t>阿罗拉穿山王</t>
+  </si>
+  <si>
+    <t>阿罗拉六尾</t>
+  </si>
+  <si>
+    <t>阿罗拉九尾</t>
+  </si>
+  <si>
+    <t>阿罗拉地鼠</t>
+  </si>
+  <si>
+    <t>阿罗拉三地鼠</t>
+  </si>
+  <si>
+    <t>阿罗拉喵喵</t>
+  </si>
+  <si>
+    <t>阿罗拉猫老大</t>
+  </si>
+  <si>
+    <t>阿罗拉小拳石</t>
+  </si>
+  <si>
+    <t>阿罗拉隆隆石</t>
+  </si>
+  <si>
+    <t>阿罗拉隆隆岩</t>
+  </si>
+  <si>
+    <t>阿罗拉臭泥</t>
+  </si>
+  <si>
+    <t>阿罗拉臭臭泥</t>
+  </si>
+  <si>
+    <t>阿罗拉椰蛋树</t>
+  </si>
+  <si>
+    <t>阿罗拉嘎啦嘎啦</t>
   </si>
 </sst>
 </file>
@@ -577,872 +693,987 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M24"/>
+  <dimension ref="A1:O24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L1" sqref="L1"/>
+    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="O2" sqref="O2:O19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <sheetData>
-    <row r="1" spans="1:13">
+    <row r="1" spans="1:15">
       <c r="A1" t="s">
         <v>10</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="B1" t="s">
+        <v>43</v>
+      </c>
+      <c r="C1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="D1" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="E1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="F1" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="4" t="s">
+      <c r="G1" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="4" t="s">
+      <c r="H1" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="4" t="s">
+      <c r="I1" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="I1" s="3" t="s">
+      <c r="J1" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="J1" s="3" t="s">
+      <c r="K1" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="K1" s="3" t="s">
+      <c r="L1" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="L1" s="3" t="s">
+      <c r="M1" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="M1" s="3" t="s">
+      <c r="N1" s="3" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="2" spans="1:13">
+      <c r="O1" s="3" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15">
       <c r="A2">
         <v>19</v>
       </c>
-      <c r="B2" s="2">
+      <c r="B2" t="s">
+        <v>44</v>
+      </c>
+      <c r="C2" s="2">
         <v>30</v>
       </c>
-      <c r="C2" s="2">
+      <c r="D2" s="2">
         <v>56</v>
       </c>
-      <c r="D2" s="2">
+      <c r="E2" s="2">
         <v>35</v>
       </c>
-      <c r="E2" s="2">
+      <c r="F2" s="2">
         <v>25</v>
       </c>
-      <c r="F2" s="2">
+      <c r="G2" s="2">
         <v>35</v>
       </c>
-      <c r="G2" s="2">
+      <c r="H2" s="2">
         <v>72</v>
       </c>
-      <c r="H2">
-        <f>SUM(B2:G2)</f>
+      <c r="I2">
+        <f>SUM(C2:H2)</f>
         <v>253</v>
       </c>
-      <c r="I2" s="3">
-        <f>2*B2</f>
+      <c r="J2" s="3">
+        <f>2*C2</f>
         <v>60</v>
       </c>
-      <c r="J2" s="3">
-        <f>ROUND((1+(G2-75)/500)*(ROUND(0.25*(7*MAX(E2,C2)+MIN(E2,C2)),0)),0)</f>
+      <c r="K2" s="3">
+        <f>ROUND((1+(H2-75)/500)*(ROUND(0.25*(7*MAX(F2,D2)+MIN(F2,D2)),0)),0)</f>
         <v>103</v>
       </c>
-      <c r="K2" s="3">
-        <f>ROUND((1+(G2-75)/500)*(ROUND(0.25*(7*MAX(F2,D2)+MIN(F2,D2)),0)),0)</f>
+      <c r="L2" s="3">
+        <f>ROUND((1+(H2-75)/500)*(ROUND(0.25*(7*MAX(G2,E2)+MIN(G2,E2)),0)),0)</f>
         <v>70</v>
       </c>
-      <c r="L2" t="s">
+      <c r="M2" t="s">
         <v>12</v>
       </c>
-      <c r="M2" t="s">
+      <c r="N2" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="3" spans="1:13">
+      <c r="O2" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15">
       <c r="A3">
         <v>20</v>
       </c>
-      <c r="B3" s="2">
+      <c r="B3" t="s">
+        <v>45</v>
+      </c>
+      <c r="C3" s="2">
         <v>75</v>
       </c>
-      <c r="C3" s="2">
+      <c r="D3" s="2">
         <v>71</v>
       </c>
-      <c r="D3" s="2">
+      <c r="E3" s="2">
         <v>70</v>
       </c>
-      <c r="E3" s="2">
+      <c r="F3" s="2">
         <v>40</v>
       </c>
-      <c r="F3" s="2">
+      <c r="G3" s="2">
         <v>80</v>
       </c>
-      <c r="G3" s="2">
+      <c r="H3" s="2">
         <v>77</v>
       </c>
-      <c r="H3">
-        <f t="shared" ref="H3:H19" si="0">SUM(B3:G3)</f>
+      <c r="I3">
+        <f t="shared" ref="I3:I19" si="0">SUM(C3:H3)</f>
         <v>413</v>
       </c>
-      <c r="I3" s="3">
-        <f t="shared" ref="I3:I19" si="1">2*B3</f>
+      <c r="J3" s="3">
+        <f t="shared" ref="J3:J19" si="1">2*C3</f>
         <v>150</v>
       </c>
-      <c r="J3" s="3">
-        <f t="shared" ref="J3:J19" si="2">ROUND((1+(G3-75)/500)*(ROUND(0.25*(7*MAX(E3,C3)+MIN(E3,C3)),0)),0)</f>
+      <c r="K3" s="3">
+        <f t="shared" ref="K3:K19" si="2">ROUND((1+(H3-75)/500)*(ROUND(0.25*(7*MAX(F3,D3)+MIN(F3,D3)),0)),0)</f>
         <v>135</v>
       </c>
-      <c r="K3" s="3">
-        <f t="shared" ref="K3:K19" si="3">ROUND((1+(G3-75)/500)*(ROUND(0.25*(7*MAX(F3,D3)+MIN(F3,D3)),0)),0)</f>
+      <c r="L3" s="3">
+        <f t="shared" ref="L3:L19" si="3">ROUND((1+(H3-75)/500)*(ROUND(0.25*(7*MAX(G3,E3)+MIN(G3,E3)),0)),0)</f>
         <v>159</v>
       </c>
-      <c r="L3" t="s">
+      <c r="M3" t="s">
         <v>12</v>
       </c>
-      <c r="M3" t="s">
+      <c r="N3" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="4" spans="1:13">
+      <c r="O3" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15">
       <c r="A4">
         <v>26</v>
       </c>
-      <c r="B4" s="2">
+      <c r="B4" t="s">
+        <v>46</v>
+      </c>
+      <c r="C4" s="2">
         <v>60</v>
       </c>
-      <c r="C4" s="2">
+      <c r="D4" s="2">
         <v>85</v>
       </c>
-      <c r="D4" s="2">
+      <c r="E4" s="2">
         <v>50</v>
       </c>
-      <c r="E4" s="2">
+      <c r="F4" s="2">
         <v>95</v>
       </c>
-      <c r="F4" s="2">
+      <c r="G4" s="2">
         <v>85</v>
       </c>
-      <c r="G4" s="2">
+      <c r="H4" s="2">
         <v>110</v>
       </c>
-      <c r="H4">
+      <c r="I4">
         <f t="shared" si="0"/>
         <v>485</v>
       </c>
-      <c r="I4" s="3">
+      <c r="J4" s="3">
         <f t="shared" si="1"/>
         <v>120</v>
       </c>
-      <c r="J4" s="3">
+      <c r="K4" s="3">
         <f t="shared" si="2"/>
         <v>201</v>
       </c>
-      <c r="K4" s="3">
+      <c r="L4" s="3">
         <f t="shared" si="3"/>
         <v>172</v>
       </c>
-      <c r="L4" t="s">
+      <c r="M4" t="s">
         <v>13</v>
       </c>
-      <c r="M4" t="s">
+      <c r="N4" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="5" spans="1:13">
+      <c r="O4" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15">
       <c r="A5">
         <v>27</v>
       </c>
-      <c r="B5" s="2">
+      <c r="B5" t="s">
+        <v>47</v>
+      </c>
+      <c r="C5" s="2">
         <v>50</v>
       </c>
-      <c r="C5" s="2">
+      <c r="D5" s="2">
         <v>75</v>
       </c>
-      <c r="D5" s="2">
+      <c r="E5" s="2">
         <v>90</v>
       </c>
-      <c r="E5" s="2">
+      <c r="F5" s="2">
         <v>10</v>
       </c>
-      <c r="F5" s="2">
+      <c r="G5" s="2">
         <v>35</v>
       </c>
-      <c r="G5" s="2">
+      <c r="H5" s="2">
         <v>40</v>
       </c>
-      <c r="H5">
+      <c r="I5">
         <f t="shared" si="0"/>
         <v>300</v>
       </c>
-      <c r="I5" s="3">
+      <c r="J5" s="3">
         <f t="shared" si="1"/>
         <v>100</v>
       </c>
-      <c r="J5" s="3">
+      <c r="K5" s="3">
         <f t="shared" si="2"/>
         <v>125</v>
       </c>
-      <c r="K5" s="3">
+      <c r="L5" s="3">
         <f t="shared" si="3"/>
         <v>154</v>
       </c>
-      <c r="L5" t="s">
+      <c r="M5" t="s">
         <v>14</v>
       </c>
-      <c r="M5" t="s">
+      <c r="N5" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="6" spans="1:13">
+      <c r="O5" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15">
       <c r="A6">
         <v>28</v>
       </c>
-      <c r="B6" s="2">
+      <c r="B6" t="s">
+        <v>48</v>
+      </c>
+      <c r="C6" s="2">
         <v>75</v>
       </c>
-      <c r="C6" s="2">
+      <c r="D6" s="2">
         <v>100</v>
       </c>
-      <c r="D6" s="2">
+      <c r="E6" s="2">
         <v>120</v>
       </c>
-      <c r="E6" s="2">
+      <c r="F6" s="2">
         <v>25</v>
-      </c>
-      <c r="F6" s="2">
-        <v>65</v>
       </c>
       <c r="G6" s="2">
         <v>65</v>
       </c>
-      <c r="H6">
+      <c r="H6" s="2">
+        <v>65</v>
+      </c>
+      <c r="I6">
         <f t="shared" si="0"/>
         <v>450</v>
       </c>
-      <c r="I6" s="3">
+      <c r="J6" s="3">
         <f t="shared" si="1"/>
         <v>150</v>
       </c>
-      <c r="J6" s="3">
+      <c r="K6" s="3">
         <f t="shared" si="2"/>
         <v>177</v>
       </c>
-      <c r="K6" s="3">
+      <c r="L6" s="3">
         <f t="shared" si="3"/>
         <v>221</v>
       </c>
-      <c r="L6" t="s">
+      <c r="M6" t="s">
         <v>14</v>
       </c>
-      <c r="M6" t="s">
+      <c r="N6" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="7" spans="1:13">
+      <c r="O6" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15">
       <c r="A7">
         <v>37</v>
       </c>
-      <c r="B7" s="2">
+      <c r="B7" t="s">
+        <v>49</v>
+      </c>
+      <c r="C7" s="2">
         <v>38</v>
       </c>
-      <c r="C7" s="2">
+      <c r="D7" s="2">
         <v>41</v>
       </c>
-      <c r="D7" s="2">
+      <c r="E7" s="2">
         <v>40</v>
       </c>
-      <c r="E7" s="2">
+      <c r="F7" s="2">
         <v>50</v>
-      </c>
-      <c r="F7" s="2">
-        <v>65</v>
       </c>
       <c r="G7" s="2">
         <v>65</v>
       </c>
-      <c r="H7">
+      <c r="H7" s="2">
+        <v>65</v>
+      </c>
+      <c r="I7">
         <f t="shared" si="0"/>
         <v>299</v>
       </c>
-      <c r="I7" s="3">
+      <c r="J7" s="3">
         <f t="shared" si="1"/>
         <v>76</v>
       </c>
-      <c r="J7" s="3">
+      <c r="K7" s="3">
         <f t="shared" si="2"/>
         <v>96</v>
       </c>
-      <c r="K7" s="3">
+      <c r="L7" s="3">
         <f t="shared" si="3"/>
         <v>122</v>
       </c>
-      <c r="L7" t="s">
+      <c r="M7" t="s">
         <v>15</v>
       </c>
-      <c r="M7" t="s">
+      <c r="N7" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="8" spans="1:13">
+      <c r="O7" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15">
       <c r="A8">
         <v>38</v>
       </c>
-      <c r="B8" s="2">
+      <c r="B8" t="s">
+        <v>50</v>
+      </c>
+      <c r="C8" s="2">
         <v>73</v>
       </c>
-      <c r="C8" s="2">
+      <c r="D8" s="2">
         <v>67</v>
       </c>
-      <c r="D8" s="2">
+      <c r="E8" s="2">
         <v>75</v>
       </c>
-      <c r="E8" s="2">
+      <c r="F8" s="2">
         <v>81</v>
       </c>
-      <c r="F8" s="2">
+      <c r="G8" s="2">
         <v>100</v>
       </c>
-      <c r="G8" s="2">
+      <c r="H8" s="2">
         <v>109</v>
       </c>
-      <c r="H8">
+      <c r="I8">
         <f t="shared" si="0"/>
         <v>505</v>
       </c>
-      <c r="I8" s="3">
+      <c r="J8" s="3">
         <f t="shared" si="1"/>
         <v>146</v>
       </c>
-      <c r="J8" s="3">
+      <c r="K8" s="3">
         <f t="shared" si="2"/>
         <v>170</v>
       </c>
-      <c r="K8" s="3">
+      <c r="L8" s="3">
         <f t="shared" si="3"/>
         <v>207</v>
       </c>
-      <c r="L8" t="s">
+      <c r="M8" t="s">
         <v>16</v>
       </c>
-      <c r="M8" t="s">
+      <c r="N8" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="9" spans="1:13">
+      <c r="O8" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15">
       <c r="A9">
         <v>50</v>
       </c>
-      <c r="B9" s="2">
+      <c r="B9" t="s">
+        <v>51</v>
+      </c>
+      <c r="C9" s="2">
         <v>10</v>
       </c>
-      <c r="C9" s="2">
+      <c r="D9" s="2">
         <v>55</v>
       </c>
-      <c r="D9" s="2">
+      <c r="E9" s="2">
         <v>30</v>
       </c>
-      <c r="E9" s="2">
+      <c r="F9" s="2">
         <v>35</v>
       </c>
-      <c r="F9" s="2">
+      <c r="G9" s="2">
         <v>45</v>
       </c>
-      <c r="G9" s="2">
+      <c r="H9" s="2">
         <v>90</v>
       </c>
-      <c r="H9">
+      <c r="I9">
         <f t="shared" si="0"/>
         <v>265</v>
       </c>
-      <c r="I9" s="3">
+      <c r="J9" s="3">
         <f t="shared" si="1"/>
         <v>20</v>
       </c>
-      <c r="J9" s="3">
+      <c r="K9" s="3">
         <f t="shared" si="2"/>
         <v>108</v>
       </c>
-      <c r="K9" s="3">
+      <c r="L9" s="3">
         <f t="shared" si="3"/>
         <v>89</v>
       </c>
-      <c r="L9" t="s">
+      <c r="M9" t="s">
         <v>17</v>
       </c>
-      <c r="M9" t="s">
+      <c r="N9" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="10" spans="1:13">
+      <c r="O9" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15">
       <c r="A10">
         <v>51</v>
       </c>
-      <c r="B10" s="2">
+      <c r="B10" t="s">
+        <v>52</v>
+      </c>
+      <c r="C10" s="2">
         <v>35</v>
       </c>
-      <c r="C10" s="2">
+      <c r="D10" s="2">
         <v>100</v>
       </c>
-      <c r="D10" s="2">
+      <c r="E10" s="2">
         <v>60</v>
       </c>
-      <c r="E10" s="2">
+      <c r="F10" s="2">
         <v>50</v>
       </c>
-      <c r="F10" s="2">
+      <c r="G10" s="2">
         <v>70</v>
       </c>
-      <c r="G10" s="2">
+      <c r="H10" s="2">
         <v>110</v>
       </c>
-      <c r="H10">
+      <c r="I10">
         <f t="shared" si="0"/>
         <v>425</v>
       </c>
-      <c r="I10" s="3">
+      <c r="J10" s="3">
         <f t="shared" si="1"/>
         <v>70</v>
       </c>
-      <c r="J10" s="3">
+      <c r="K10" s="3">
         <f t="shared" si="2"/>
         <v>201</v>
       </c>
-      <c r="K10" s="3">
+      <c r="L10" s="3">
         <f t="shared" si="3"/>
         <v>148</v>
       </c>
-      <c r="L10" t="s">
+      <c r="M10" t="s">
         <v>17</v>
       </c>
-      <c r="M10" t="s">
+      <c r="N10" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="11" spans="1:13">
+      <c r="O10" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15">
       <c r="A11">
         <v>52</v>
       </c>
-      <c r="B11" s="2">
+      <c r="B11" t="s">
+        <v>53</v>
+      </c>
+      <c r="C11" s="2">
         <v>40</v>
-      </c>
-      <c r="C11" s="2">
-        <v>35</v>
       </c>
       <c r="D11" s="2">
         <v>35</v>
       </c>
       <c r="E11" s="2">
+        <v>35</v>
+      </c>
+      <c r="F11" s="2">
         <v>50</v>
       </c>
-      <c r="F11" s="2">
+      <c r="G11" s="2">
         <v>40</v>
       </c>
-      <c r="G11" s="2">
+      <c r="H11" s="2">
         <v>90</v>
       </c>
-      <c r="H11">
+      <c r="I11">
         <f t="shared" si="0"/>
         <v>290</v>
       </c>
-      <c r="I11" s="3">
+      <c r="J11" s="3">
         <f t="shared" si="1"/>
         <v>80</v>
       </c>
-      <c r="J11" s="3">
+      <c r="K11" s="3">
         <f t="shared" si="2"/>
         <v>99</v>
       </c>
-      <c r="K11" s="3">
+      <c r="L11" s="3">
         <f t="shared" si="3"/>
         <v>81</v>
       </c>
-      <c r="L11" t="s">
+      <c r="M11" t="s">
         <v>18</v>
       </c>
-      <c r="M11" t="s">
+      <c r="N11" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="12" spans="1:13">
+      <c r="O11" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15">
       <c r="A12">
         <v>53</v>
       </c>
-      <c r="B12" s="2">
+      <c r="B12" t="s">
+        <v>54</v>
+      </c>
+      <c r="C12" s="2">
         <v>65</v>
-      </c>
-      <c r="C12" s="2">
-        <v>60</v>
       </c>
       <c r="D12" s="2">
         <v>60</v>
       </c>
       <c r="E12" s="2">
+        <v>60</v>
+      </c>
+      <c r="F12" s="2">
         <v>75</v>
       </c>
-      <c r="F12" s="2">
+      <c r="G12" s="2">
         <v>65</v>
       </c>
-      <c r="G12" s="2">
+      <c r="H12" s="2">
         <v>115</v>
       </c>
-      <c r="H12">
+      <c r="I12">
         <f t="shared" si="0"/>
         <v>440</v>
       </c>
-      <c r="I12" s="3">
+      <c r="J12" s="3">
         <f t="shared" si="1"/>
         <v>130</v>
       </c>
-      <c r="J12" s="3">
+      <c r="K12" s="3">
         <f t="shared" si="2"/>
         <v>158</v>
       </c>
-      <c r="K12" s="3">
+      <c r="L12" s="3">
         <f t="shared" si="3"/>
         <v>139</v>
       </c>
-      <c r="L12" t="s">
+      <c r="M12" t="s">
         <v>18</v>
       </c>
-      <c r="M12" t="s">
+      <c r="N12" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="13" spans="1:13">
+      <c r="O12" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15">
       <c r="A13">
         <v>74</v>
       </c>
-      <c r="B13" s="2">
+      <c r="B13" t="s">
+        <v>55</v>
+      </c>
+      <c r="C13" s="2">
         <v>40</v>
       </c>
-      <c r="C13" s="2">
+      <c r="D13" s="2">
         <v>80</v>
       </c>
-      <c r="D13" s="2">
+      <c r="E13" s="2">
         <v>100</v>
-      </c>
-      <c r="E13" s="2">
-        <v>30</v>
       </c>
       <c r="F13" s="2">
         <v>30</v>
       </c>
       <c r="G13" s="2">
+        <v>30</v>
+      </c>
+      <c r="H13" s="2">
         <v>20</v>
       </c>
-      <c r="H13">
+      <c r="I13">
         <f t="shared" si="0"/>
         <v>300</v>
       </c>
-      <c r="I13" s="3">
+      <c r="J13" s="3">
         <f t="shared" si="1"/>
         <v>80</v>
       </c>
-      <c r="J13" s="3">
+      <c r="K13" s="3">
         <f t="shared" si="2"/>
         <v>132</v>
       </c>
-      <c r="K13" s="3">
+      <c r="L13" s="3">
         <f t="shared" si="3"/>
         <v>163</v>
       </c>
-      <c r="L13" t="s">
+      <c r="M13" t="s">
         <v>19</v>
       </c>
-      <c r="M13" t="s">
+      <c r="N13" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="14" spans="1:13">
+      <c r="O13" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15">
       <c r="A14">
         <v>75</v>
       </c>
-      <c r="B14" s="2">
+      <c r="B14" t="s">
+        <v>56</v>
+      </c>
+      <c r="C14" s="2">
         <v>55</v>
       </c>
-      <c r="C14" s="2">
+      <c r="D14" s="2">
         <v>95</v>
       </c>
-      <c r="D14" s="2">
+      <c r="E14" s="2">
         <v>115</v>
-      </c>
-      <c r="E14" s="2">
-        <v>45</v>
       </c>
       <c r="F14" s="2">
         <v>45</v>
       </c>
       <c r="G14" s="2">
+        <v>45</v>
+      </c>
+      <c r="H14" s="2">
         <v>35</v>
       </c>
-      <c r="H14">
+      <c r="I14">
         <f t="shared" si="0"/>
         <v>390</v>
       </c>
-      <c r="I14" s="3">
+      <c r="J14" s="3">
         <f t="shared" si="1"/>
         <v>110</v>
       </c>
-      <c r="J14" s="3">
+      <c r="K14" s="3">
         <f t="shared" si="2"/>
         <v>164</v>
       </c>
-      <c r="K14" s="3">
+      <c r="L14" s="3">
         <f t="shared" si="3"/>
         <v>196</v>
       </c>
-      <c r="L14" t="s">
+      <c r="M14" t="s">
         <v>19</v>
       </c>
-      <c r="M14" t="s">
+      <c r="N14" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="15" spans="1:13">
+      <c r="O14" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15">
       <c r="A15">
         <v>76</v>
       </c>
-      <c r="B15" s="2">
+      <c r="B15" t="s">
+        <v>57</v>
+      </c>
+      <c r="C15" s="2">
         <v>80</v>
       </c>
-      <c r="C15" s="2">
+      <c r="D15" s="2">
         <v>120</v>
       </c>
-      <c r="D15" s="2">
+      <c r="E15" s="2">
         <v>130</v>
       </c>
-      <c r="E15" s="2">
+      <c r="F15" s="2">
         <v>55</v>
       </c>
-      <c r="F15" s="2">
+      <c r="G15" s="2">
         <v>65</v>
       </c>
-      <c r="G15" s="2">
+      <c r="H15" s="2">
         <v>45</v>
       </c>
-      <c r="H15">
+      <c r="I15">
         <f t="shared" si="0"/>
         <v>495</v>
       </c>
-      <c r="I15" s="3">
+      <c r="J15" s="3">
         <f t="shared" si="1"/>
         <v>160</v>
       </c>
-      <c r="J15" s="3">
+      <c r="K15" s="3">
         <f t="shared" si="2"/>
         <v>211</v>
       </c>
-      <c r="K15" s="3">
+      <c r="L15" s="3">
         <f t="shared" si="3"/>
         <v>229</v>
       </c>
-      <c r="L15" t="s">
+      <c r="M15" t="s">
         <v>19</v>
       </c>
-      <c r="M15" t="s">
+      <c r="N15" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="16" spans="1:13">
+      <c r="O15" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="16" spans="1:15">
       <c r="A16">
         <v>88</v>
       </c>
-      <c r="B16" s="2">
-        <v>80</v>
+      <c r="B16" t="s">
+        <v>58</v>
       </c>
       <c r="C16" s="2">
         <v>80</v>
       </c>
       <c r="D16" s="2">
+        <v>80</v>
+      </c>
+      <c r="E16" s="2">
         <v>50</v>
       </c>
-      <c r="E16" s="2">
+      <c r="F16" s="2">
         <v>40</v>
       </c>
-      <c r="F16" s="2">
+      <c r="G16" s="2">
         <v>50</v>
       </c>
-      <c r="G16" s="2">
+      <c r="H16" s="2">
         <v>25</v>
       </c>
-      <c r="H16">
+      <c r="I16">
         <f t="shared" si="0"/>
         <v>325</v>
       </c>
-      <c r="I16" s="3">
+      <c r="J16" s="3">
         <f t="shared" si="1"/>
         <v>160</v>
       </c>
-      <c r="J16" s="3">
+      <c r="K16" s="3">
         <f t="shared" si="2"/>
         <v>135</v>
       </c>
-      <c r="K16" s="3">
+      <c r="L16" s="3">
         <f t="shared" si="3"/>
         <v>90</v>
       </c>
-      <c r="L16" t="s">
+      <c r="M16" t="s">
         <v>20</v>
       </c>
-      <c r="M16" t="s">
+      <c r="N16" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="17" spans="1:13">
+      <c r="O16" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="17" spans="1:15">
       <c r="A17">
         <v>89</v>
       </c>
-      <c r="B17" s="2">
-        <v>105</v>
+      <c r="B17" t="s">
+        <v>59</v>
       </c>
       <c r="C17" s="2">
         <v>105</v>
       </c>
       <c r="D17" s="2">
+        <v>105</v>
+      </c>
+      <c r="E17" s="2">
         <v>75</v>
       </c>
-      <c r="E17" s="2">
+      <c r="F17" s="2">
         <v>65</v>
       </c>
-      <c r="F17" s="2">
+      <c r="G17" s="2">
         <v>100</v>
       </c>
-      <c r="G17" s="2">
+      <c r="H17" s="2">
         <v>50</v>
       </c>
-      <c r="H17">
+      <c r="I17">
         <f t="shared" si="0"/>
         <v>500</v>
       </c>
-      <c r="I17" s="3">
+      <c r="J17" s="3">
         <f t="shared" si="1"/>
         <v>210</v>
       </c>
-      <c r="J17" s="3">
+      <c r="K17" s="3">
         <f t="shared" si="2"/>
         <v>190</v>
       </c>
-      <c r="K17" s="3">
+      <c r="L17" s="3">
         <f t="shared" si="3"/>
         <v>184</v>
       </c>
-      <c r="L17" t="s">
+      <c r="M17" t="s">
         <v>20</v>
       </c>
-      <c r="M17" t="s">
+      <c r="N17" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="18" spans="1:13">
+      <c r="O17" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="18" spans="1:15">
       <c r="A18">
         <v>103</v>
       </c>
-      <c r="B18" s="2">
+      <c r="B18" t="s">
+        <v>60</v>
+      </c>
+      <c r="C18" s="2">
         <v>95</v>
       </c>
-      <c r="C18" s="2">
+      <c r="D18" s="2">
         <v>105</v>
       </c>
-      <c r="D18" s="2">
+      <c r="E18" s="2">
         <v>85</v>
       </c>
-      <c r="E18" s="2">
+      <c r="F18" s="2">
         <v>125</v>
       </c>
-      <c r="F18" s="2">
+      <c r="G18" s="2">
         <v>75</v>
       </c>
-      <c r="G18" s="2">
+      <c r="H18" s="2">
         <v>45</v>
       </c>
-      <c r="H18">
+      <c r="I18">
         <f t="shared" si="0"/>
         <v>530</v>
       </c>
-      <c r="I18" s="3">
+      <c r="J18" s="3">
         <f t="shared" si="1"/>
         <v>190</v>
       </c>
-      <c r="J18" s="3">
+      <c r="K18" s="3">
         <f t="shared" si="2"/>
         <v>230</v>
       </c>
-      <c r="K18" s="3">
+      <c r="L18" s="3">
         <f t="shared" si="3"/>
         <v>158</v>
       </c>
-      <c r="L18" t="s">
+      <c r="M18" t="s">
         <v>21</v>
       </c>
-      <c r="M18" t="s">
+      <c r="N18" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="19" spans="1:13">
+      <c r="O18" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="19" spans="1:15">
       <c r="A19">
         <v>105</v>
       </c>
-      <c r="B19" s="2">
+      <c r="B19" t="s">
+        <v>61</v>
+      </c>
+      <c r="C19" s="2">
         <v>60</v>
       </c>
-      <c r="C19" s="2">
+      <c r="D19" s="2">
         <v>80</v>
       </c>
-      <c r="D19" s="2">
+      <c r="E19" s="2">
         <v>110</v>
       </c>
-      <c r="E19" s="2">
+      <c r="F19" s="2">
         <v>50</v>
       </c>
-      <c r="F19" s="2">
+      <c r="G19" s="2">
         <v>80</v>
       </c>
-      <c r="G19" s="2">
+      <c r="H19" s="2">
         <v>45</v>
       </c>
-      <c r="H19">
+      <c r="I19">
         <f t="shared" si="0"/>
         <v>425</v>
       </c>
-      <c r="I19" s="3">
+      <c r="J19" s="3">
         <f t="shared" si="1"/>
         <v>120</v>
       </c>
-      <c r="J19" s="3">
+      <c r="K19" s="3">
         <f t="shared" si="2"/>
         <v>144</v>
       </c>
-      <c r="K19" s="3">
+      <c r="L19" s="3">
         <f t="shared" si="3"/>
         <v>200</v>
       </c>
-      <c r="L19" t="s">
+      <c r="M19" t="s">
         <v>22</v>
       </c>
-      <c r="M19" t="s">
+      <c r="N19" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="24" spans="1:13">
+      <c r="O19" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="24" spans="1:15">
       <c r="A24" s="1"/>
       <c r="B24" s="1"/>
       <c r="C24" s="1"/>
       <c r="D24" s="1"/>
       <c r="E24" s="1"/>
       <c r="F24" s="1"/>
+      <c r="G24" s="1"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>

</xml_diff>